<commit_message>
Final self-report PCSS and TARF added
</commit_message>
<xml_diff>
--- a/data/KAHI_pcss.xlsx
+++ b/data/KAHI_pcss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFBE39A-DF2D-7146-B0A9-E26D5EB6DACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B63013-F44F-F342-8320-3F02F9B9C306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="780" windowWidth="27240" windowHeight="15300" xr2:uid="{CEE72CA0-3CC1-E94C-A911-68D3D778F2D1}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +521,9 @@
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -530,6 +533,9 @@
         <v>4</v>
       </c>
       <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
     </row>
@@ -543,6 +549,9 @@
       <c r="C4">
         <v>3</v>
       </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -554,6 +563,9 @@
       <c r="C5">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -565,6 +577,9 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -576,6 +591,9 @@
       <c r="C7">
         <v>5</v>
       </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -587,6 +605,9 @@
       <c r="C8">
         <v>3</v>
       </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -598,6 +619,9 @@
       <c r="C9">
         <v>4</v>
       </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -609,6 +633,9 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -620,6 +647,9 @@
       <c r="C11">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -631,6 +661,9 @@
       <c r="C12">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -642,6 +675,9 @@
       <c r="C13">
         <v>3</v>
       </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -653,6 +689,9 @@
       <c r="C14">
         <v>4</v>
       </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -664,6 +703,9 @@
       <c r="C15">
         <v>5</v>
       </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -675,8 +717,11 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -686,8 +731,11 @@
       <c r="C17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -697,8 +745,11 @@
       <c r="C18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -708,8 +759,11 @@
       <c r="C19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -719,8 +773,11 @@
       <c r="C20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -730,8 +787,11 @@
       <c r="C21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -741,8 +801,11 @@
       <c r="C22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -752,8 +815,11 @@
       <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -765,8 +831,12 @@
         <f>SUM(C2:C23)</f>
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f>SUM(D2:D23)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -778,8 +848,12 @@
         <f>SUM(C2 + C12 + C13)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f>SUM(D2 + D12 + D13)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -791,8 +865,12 @@
         <f>SUM(C19:C22)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f>SUM(D19:D22)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -804,8 +882,12 @@
         <f>SUM(C14:C18)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f>SUM(D14:D18)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -817,8 +899,12 @@
         <f>C23</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f>D23</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -830,8 +916,12 @@
         <f>SUM(C3:C6)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f>SUM(D3:D6)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -842,6 +932,10 @@
       <c r="C30">
         <f>SUM(C7:C11)</f>
         <v>16</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D7:D11)</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>